<commit_message>
search based scraping done
</commit_message>
<xml_diff>
--- a/leads_scored.xlsx
+++ b/leads_scored.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,25 +430,25 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>The Mark Boulevard</v>
+        <v>cult.fit</v>
       </c>
       <c r="B2" t="str">
-        <v>info@themarkboulevard.com</v>
+        <v>hello@cult.fit</v>
       </c>
       <c r="C2" t="str">
-        <v>http://www.themarkboulevard.com/</v>
+        <v>https://www.cure.fit/</v>
       </c>
       <c r="D2" t="str">
-        <v>restaurant</v>
+        <v>gym</v>
       </c>
       <c r="E2" t="str">
-        <v>EPIP Zone, Whitefield</v>
+        <v>bengaluru</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G2" t="str">
-        <v>COLD_LEAD</v>
+        <v>WARM_LEAD</v>
       </c>
       <c r="H2" t="str">
         <v>PENDING</v>
@@ -456,19 +456,19 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Adyar Ananda Bhavan</v>
+        <v>WE Fitness, Health and Wellness Center</v>
       </c>
       <c r="B3" t="str">
-        <v>care@aabsweets.com</v>
+        <v>wefitnessblr@gmail.com</v>
       </c>
       <c r="C3" t="str">
-        <v>https://aabsweets.com</v>
+        <v>https://wefithealth.com/</v>
       </c>
       <c r="D3" t="str">
-        <v>restaurant</v>
+        <v>gym</v>
       </c>
       <c r="E3" t="str">
-        <v>Whitefield Main Road</v>
+        <v>23rd Main Rd, Nagaraja Garden, J P Nagar Phase 5, JP Nagar, bengaluru</v>
       </c>
       <c r="F3">
         <v>15</v>
@@ -482,22 +482,22 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Cloud Nine Hospital</v>
+        <v>i-fitness</v>
       </c>
       <c r="B4" t="str">
-        <v>info@cloudninecare.com</v>
+        <v>info@i-fitness.in</v>
       </c>
       <c r="C4" t="str">
-        <v>https://cloudninecare.com/</v>
+        <v>https://i-fitness.in/</v>
       </c>
       <c r="D4" t="str">
-        <v>hospital</v>
+        <v>gym</v>
       </c>
       <c r="E4" t="str">
-        <v>Whitefield Main Road</v>
+        <v>Chabria Square, KH Road, Bhadrappa Layout, Srinivas Colony, Sudhama Nagar,, bengaluru</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G4" t="str">
         <v>COLD_LEAD</v>
@@ -508,25 +508,25 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Chinita</v>
+        <v>The Fitness Zone</v>
       </c>
       <c r="B5" t="str">
-        <v>contact@chinita.in</v>
+        <v>you@example.com</v>
       </c>
       <c r="C5" t="str">
-        <v>https://www.chinita.in/</v>
+        <v>https://www.thefitnesszone.in/</v>
       </c>
       <c r="D5" t="str">
-        <v>restaurant</v>
+        <v>gym</v>
       </c>
       <c r="E5" t="str">
-        <v>Indiranagar Double Road</v>
+        <v>1st Main, 4th Cross, Maruthi Nagar, Near-RS High School, Madiwala, Chikka Madivala, 1st Stage, BTM Layout, bengaluru</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G5" t="str">
-        <v>COLD_LEAD</v>
+        <v>WARM_LEAD</v>
       </c>
       <c r="H5" t="str">
         <v>PENDING</v>
@@ -534,25 +534,25 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Gulecha Dental Care</v>
+        <v>Bodycraft Academy</v>
       </c>
       <c r="B6" t="str">
-        <v>clinic@gulechadental.com</v>
+        <v>guestrelations@bodycraft.co.in</v>
       </c>
       <c r="C6" t="str">
-        <v>https://www.gulechadental.com/</v>
+        <v>https://www.bodycraft.co.in/</v>
       </c>
       <c r="D6" t="str">
-        <v>hospital</v>
+        <v>gym</v>
       </c>
       <c r="E6" t="str">
-        <v>4th Cross Road, KV Layout, Jayanagar 4th Block</v>
+        <v>Ganapathi Temple Road,7th Block, Koramangala, bengaluru</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G6" t="str">
-        <v>COLD_LEAD</v>
+        <v>WARM_LEAD</v>
       </c>
       <c r="H6" t="str">
         <v>PENDING</v>
@@ -560,19 +560,19 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Garden By Su</v>
+        <v>Chisel Fitness Center</v>
       </c>
       <c r="B7" t="str">
-        <v>hello@gardenbysu.com</v>
+        <v>flags@2x.png</v>
       </c>
       <c r="C7" t="str">
-        <v>https://www.gardenbysu.com/</v>
+        <v>https://chisel.co.in/</v>
       </c>
       <c r="D7" t="str">
-        <v>restaurant</v>
+        <v>gym</v>
       </c>
       <c r="E7" t="str">
-        <v>9th Main, 46th Cross Rd, 5th Block, Jayanagar</v>
+        <v>J.B Square building, Kalpana Chawala Road, Sanjay Nagar, bengaluru</v>
       </c>
       <c r="F7">
         <v>15</v>
@@ -586,19 +586,19 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Welnext</v>
+        <v>Body and Soul Fitness Academy</v>
       </c>
       <c r="B8" t="str">
-        <v>hello@welnext.com</v>
+        <v>info@bodyandsoul.org</v>
       </c>
       <c r="C8" t="str">
-        <v>https://welnext.com/</v>
+        <v>https://bodyandsoul.org/</v>
       </c>
       <c r="D8" t="str">
-        <v>hospital</v>
+        <v>gym</v>
       </c>
       <c r="E8" t="str">
-        <v>Third Floor, H.S.R Agara Circle, Sarjapura, Outer Ring Rd, Agara Village, HSR Layout,</v>
+        <v>Spice Garden Complex, Marathahalli Main Rd, Spice Garden Layout, Lakshminarayana Pura, Marathahall, bengaluru</v>
       </c>
       <c r="F8">
         <v>5</v>
@@ -612,19 +612,19 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Healing Earth Multispeciality Ayurveda Hospital</v>
+        <v>Pulse Fitness</v>
       </c>
       <c r="B9" t="str">
-        <v>20info@healingearth.co.in</v>
+        <v>contact@gympik.com</v>
       </c>
       <c r="C9" t="str">
-        <v>https://www.healingearth.co.in/</v>
+        <v>https://www.gympik.com/</v>
       </c>
       <c r="D9" t="str">
-        <v>hospital</v>
+        <v>gym</v>
       </c>
       <c r="E9" t="str">
-        <v>HSR Ring Road, 5th Sector , HSR Layout, Karnataka</v>
+        <v>Thambu Chetty Palya Main Rd, Bhadrappa Layout, M Vishveshvaraiah Nagar, Horamavu, bengaluru</v>
       </c>
       <c r="F9">
         <v>5</v>
@@ -638,25 +638,25 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Global Ayurveda Multispeciality Hospital</v>
+        <v>Impact Fitness Studio</v>
       </c>
       <c r="B10" t="str">
-        <v>20info@healingearth.co.in</v>
+        <v>impactfitness2021@gmail.com</v>
       </c>
       <c r="C10" t="str">
-        <v>https://www.healingearth.co.in/</v>
+        <v>https://www.impactfitness.in/</v>
       </c>
       <c r="D10" t="str">
-        <v>hospital</v>
+        <v>gym</v>
       </c>
       <c r="E10" t="str">
-        <v>HSR Ring Road, 5th Sector , HSR Layout, Jakkasandra, 1st Block Koramangala, HSR Layout, Karnataka</v>
+        <v>HAL 2nd Stage, Indiranagar, Bhadrappa Layout, Sodepur, Appareddipalya, Indiranagar, Bengaluru, bengaluru</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G10" t="str">
-        <v>COLD_LEAD</v>
+        <v>WARM_LEAD</v>
       </c>
       <c r="H10" t="str">
         <v>PENDING</v>
@@ -664,19 +664,19 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Lotus Diagnostic Centre</v>
+        <v>Fitness One Gym</v>
       </c>
       <c r="B11" t="str">
-        <v>lotusdiagnostic@gmail.com</v>
+        <v>info@fitnessone.in</v>
       </c>
       <c r="C11" t="str">
-        <v>https://lotusdiagnostic.com/</v>
+        <v>https://www.fitnessone.in/</v>
       </c>
       <c r="D11" t="str">
-        <v>clinic</v>
+        <v>gym</v>
       </c>
       <c r="E11" t="str">
-        <v>, CMH Road, Near ICICI Bank ATM,Indiranagar</v>
+        <v>Fitness One Brookefield, AECS Layout - C Block, AECS Layout, Brookefield,, bengaluru</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -690,25 +690,25 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Amplifon</v>
+        <v>Gold's Gym</v>
       </c>
       <c r="B12" t="str">
-        <v>amplifon-logo@3x.png</v>
+        <v>customer.care@goldsgym.in</v>
       </c>
       <c r="C12" t="str">
-        <v>https://www.amplifon.in/</v>
+        <v>https://goldsgym.in/</v>
       </c>
       <c r="D12" t="str">
-        <v>clinic</v>
+        <v>gym</v>
       </c>
       <c r="E12" t="str">
-        <v>26th Main Road, 4th T Block East, Jayanagara 9th Block</v>
+        <v>No.2631, 27th Main Road, 1st Sector, HSR Layout, Opp CPWD Complex, 1st Sector, HSR Layout, bengaluru</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G12" t="str">
-        <v>COLD_LEAD</v>
+        <v>WARM_LEAD</v>
       </c>
       <c r="H12" t="str">
         <v>PENDING</v>
@@ -716,19 +716,19 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Tommy Hilfiger</v>
+        <v>Academy of Strength</v>
       </c>
       <c r="B13" t="str">
-        <v>reportfraud@pvh.com</v>
+        <v>info@academyofstrength.in</v>
       </c>
       <c r="C13" t="str">
-        <v>http://www.global.tommy.com</v>
+        <v>https://www.academyofstrength.in/</v>
       </c>
       <c r="D13" t="str">
-        <v>clothes</v>
+        <v>gym</v>
       </c>
       <c r="E13" t="str">
-        <v>Whitefield Road</v>
+        <v>100ft Road, HAL 2nd Stage, bengaluru</v>
       </c>
       <c r="F13">
         <v>5</v>
@@ -742,25 +742,25 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Blackberrys</v>
+        <v>The Practice Room</v>
       </c>
       <c r="B14" t="str">
-        <v>customersupport@blackberrys.com</v>
+        <v>yoga@thepracticeroom.in</v>
       </c>
       <c r="C14" t="str">
-        <v>https://www.blackberrys.com/</v>
+        <v>https://thepracticeroom.in</v>
       </c>
       <c r="D14" t="str">
-        <v>clothes</v>
+        <v>gym</v>
       </c>
       <c r="E14" t="str">
-        <v>Whitefield Main Road, Mahadevpura, Devasandra Industrial Estate, Krishnarajapuram</v>
+        <v>bengaluru</v>
       </c>
       <c r="F14">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G14" t="str">
-        <v>COLD_LEAD</v>
+        <v>WARM_LEAD</v>
       </c>
       <c r="H14" t="str">
         <v>PENDING</v>
@@ -768,25 +768,25 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Copper Chimney</v>
+        <v>cult.fit</v>
       </c>
       <c r="B15" t="str">
-        <v>info@charcoalconcepts.com</v>
+        <v>hello@cult.fit</v>
       </c>
       <c r="C15" t="str">
-        <v>https://www.copperchimney.in/</v>
+        <v>https://www.cult.fit</v>
       </c>
       <c r="D15" t="str">
-        <v>restaurant</v>
+        <v>gym</v>
       </c>
       <c r="E15" t="str">
-        <v>Whitefield Main Road, Mahadevpura, Devasandra Industrial Estate, Krishnarajapuram</v>
+        <v>Swamy Vivekanandha Road, bengaluru</v>
       </c>
       <c r="F15">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G15" t="str">
-        <v>COLD_LEAD</v>
+        <v>WARM_LEAD</v>
       </c>
       <c r="H15" t="str">
         <v>PENDING</v>
@@ -794,25 +794,25 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Ed Hardy</v>
+        <v>National Academy Of Naturopathy And Yoga</v>
       </c>
       <c r="B16" t="str">
-        <v>customerservice@edhardyoriginals.com</v>
+        <v>nanyhlm@gmai.com</v>
       </c>
       <c r="C16" t="str">
-        <v>https://www.edhardyoriginals.com/</v>
+        <v>https://sahajaswasthya.com/</v>
       </c>
       <c r="D16" t="str">
-        <v>clothes</v>
+        <v>gym</v>
       </c>
       <c r="E16" t="str">
-        <v>Whitefield Main Road, Mahadevpura, Devasandra Industrial Estate, Krishnarajapuram</v>
+        <v>3rd Cross, 5th Main, bengaluru</v>
       </c>
       <c r="F16">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G16" t="str">
-        <v>COLD_LEAD</v>
+        <v>WARM_LEAD</v>
       </c>
       <c r="H16" t="str">
         <v>PENDING</v>
@@ -820,449 +820,33 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Mufti</v>
+        <v>Asana</v>
       </c>
       <c r="B17" t="str">
-        <v>support@muftijeans.in</v>
+        <v>asanagroups@gmail.com</v>
       </c>
       <c r="C17" t="str">
-        <v>https://www.muftijeans.in/</v>
+        <v>https://asanayogacafe.com/</v>
       </c>
       <c r="D17" t="str">
-        <v>clothes</v>
+        <v>gym</v>
       </c>
       <c r="E17" t="str">
-        <v>Whitefield Main Road, Mahadevpura, Devasandra Industrial Estate, Krishnarajapuram</v>
+        <v>8th Main Road, bengaluru</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G17" t="str">
-        <v>COLD_LEAD</v>
+        <v>WARM_LEAD</v>
       </c>
       <c r="H17" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>Spykar</v>
-      </c>
-      <c r="B18" t="str">
-        <v>support@starapps.studio</v>
-      </c>
-      <c r="C18" t="str">
-        <v>https://www.spykar.com/</v>
-      </c>
-      <c r="D18" t="str">
-        <v>clothes</v>
-      </c>
-      <c r="E18" t="str">
-        <v>Whitefield Road</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H18" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>Manyavar</v>
-      </c>
-      <c r="B19" t="str">
-        <v>care@vedantfashions.com</v>
-      </c>
-      <c r="C19" t="str">
-        <v>https://www.manyavar.com/</v>
-      </c>
-      <c r="D19" t="str">
-        <v>clothes</v>
-      </c>
-      <c r="E19" t="str">
-        <v>Whitefield Main Road, Mahadevpura, Devasandra Industrial Estate, Krishnarajapuram</v>
-      </c>
-      <c r="F19">
-        <v>5</v>
-      </c>
-      <c r="G19" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H19" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>Rajdhani</v>
-      </c>
-      <c r="B20" t="str">
-        <v>asset-7@4x.png</v>
-      </c>
-      <c r="C20" t="str">
-        <v>https://www.rajdhani.co.in/</v>
-      </c>
-      <c r="D20" t="str">
-        <v>restaurant</v>
-      </c>
-      <c r="E20" t="str">
-        <v>Whitefield Road</v>
-      </c>
-      <c r="F20">
-        <v>15</v>
-      </c>
-      <c r="G20" t="str">
-        <v>WARM_LEAD</v>
-      </c>
-      <c r="H20" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>Allen Solly</v>
-      </c>
-      <c r="B21" t="str">
-        <v>happytohelp@abfrl.in</v>
-      </c>
-      <c r="C21" t="str">
-        <v>https://www.allensolly.com/</v>
-      </c>
-      <c r="D21" t="str">
-        <v>clothes</v>
-      </c>
-      <c r="E21" t="str">
-        <v>Whitefield Main Road, Mahadevpura, Devasandra Industrial Estate, Krishnarajapuram</v>
-      </c>
-      <c r="F21">
-        <v>5</v>
-      </c>
-      <c r="G21" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H21" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="str">
-        <v>Van Heusen</v>
-      </c>
-      <c r="B22" t="str">
-        <v>happytohelp@abfrl.in</v>
-      </c>
-      <c r="C22" t="str">
-        <v>https://www.vanheusenindia.com/</v>
-      </c>
-      <c r="D22" t="str">
-        <v>clothes</v>
-      </c>
-      <c r="E22" t="str">
-        <v>Whitefield Main Road, Mahadevpura, Devasandra Industrial Estate, Krishnarajapuram,</v>
-      </c>
-      <c r="F22">
-        <v>5</v>
-      </c>
-      <c r="G22" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H22" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="str">
-        <v>Louis Philippe</v>
-      </c>
-      <c r="B23" t="str">
-        <v>happytohelp@abfrl.in</v>
-      </c>
-      <c r="C23" t="str">
-        <v>https://www.louisphilippe.com/</v>
-      </c>
-      <c r="D23" t="str">
-        <v>clothes</v>
-      </c>
-      <c r="E23" t="str">
-        <v>Whitefield Main Road, Mahadevpura, Devasandra Industrial Estate, Krishnarajapuram</v>
-      </c>
-      <c r="F23">
-        <v>5</v>
-      </c>
-      <c r="G23" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H23" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="str">
-        <v>Reliance Digital</v>
-      </c>
-      <c r="B24" t="str">
-        <v>3bf253eee92641789b5f905ff366df63@o71740.ingest.sentry.io</v>
-      </c>
-      <c r="C24" t="str">
-        <v>https://www.reliancedigital.in/</v>
-      </c>
-      <c r="D24" t="str">
-        <v>electronics</v>
-      </c>
-      <c r="E24" t="str">
-        <v>Whitefield Main Road, Mahadevpura, Devasandra Industrial Estate, Krishnarajapuram</v>
-      </c>
-      <c r="F24">
-        <v>5</v>
-      </c>
-      <c r="G24" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H24" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="str">
-        <v>Home town</v>
-      </c>
-      <c r="B25" t="str">
-        <v>care@hometown.in</v>
-      </c>
-      <c r="C25" t="str">
-        <v>https://www.hometown.in/</v>
-      </c>
-      <c r="D25" t="str">
-        <v>furniture</v>
-      </c>
-      <c r="E25" t="str">
-        <v>Whitefield Main Road, Mahadevpura, Devasandra Industrial Estate, Krishnarajapuram</v>
-      </c>
-      <c r="F25">
-        <v>5</v>
-      </c>
-      <c r="G25" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H25" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>Soch</v>
-      </c>
-      <c r="B26" t="str">
-        <v>support@soch.com</v>
-      </c>
-      <c r="C26" t="str">
-        <v>https://www.soch.com/in/</v>
-      </c>
-      <c r="D26" t="str">
-        <v>clothes</v>
-      </c>
-      <c r="E26" t="str">
-        <v>Whitefield Main Road, Mahadevpura, Devasandra Industrial Estate, Krishnarajapuram</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H26" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>GlobalDesi</v>
-      </c>
-      <c r="B27" t="str">
-        <v>care@globaldesi.in</v>
-      </c>
-      <c r="C27" t="str">
-        <v>https://www.globaldesi.in/</v>
-      </c>
-      <c r="D27" t="str">
-        <v>clothes</v>
-      </c>
-      <c r="E27" t="str">
-        <v>Whitefield Road</v>
-      </c>
-      <c r="F27">
-        <v>5</v>
-      </c>
-      <c r="G27" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H27" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="str">
-        <v>Shathayu Ayurveda Wellness Centre</v>
-      </c>
-      <c r="B28" t="str">
-        <v>info@shathayu.com</v>
-      </c>
-      <c r="C28" t="str">
-        <v>https://shathayu.com/</v>
-      </c>
-      <c r="D28" t="str">
-        <v>clinic</v>
-      </c>
-      <c r="E28" t="str">
-        <v>1st Floor, Sidhapura Village, Beside D-Mart, Marathahalli, Varthur Main Road, Whitefield,</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H28" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="str">
-        <v>Trust Chemist and Drugs</v>
-      </c>
-      <c r="B29" t="str">
-        <v>info@trustpharmacy.co.in</v>
-      </c>
-      <c r="C29" t="str">
-        <v>https://www.trustpharmacy.co.in/</v>
-      </c>
-      <c r="D29" t="str">
-        <v>pharmacy</v>
-      </c>
-      <c r="E29" t="str">
-        <v>Thubarahalli, Whitefield</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H29" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="str">
-        <v>Welnext</v>
-      </c>
-      <c r="B30" t="str">
-        <v>hello@welnext.com</v>
-      </c>
-      <c r="C30" t="str">
-        <v>https://welnext.com/</v>
-      </c>
-      <c r="D30" t="str">
-        <v>hospital</v>
-      </c>
-      <c r="E30" t="str">
-        <v>H.S.R Agara Circle, Sarjapura, Outer Ring Rd, Agara Village, HSR Layout</v>
-      </c>
-      <c r="F30">
-        <v>5</v>
-      </c>
-      <c r="G30" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H30" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="str">
-        <v>Columbia</v>
-      </c>
-      <c r="B31" t="str">
-        <v>dhruv.binaryic@gmail.com</v>
-      </c>
-      <c r="C31" t="str">
-        <v>https://www.columbiasportswear.co.in</v>
-      </c>
-      <c r="D31" t="str">
-        <v>clothes</v>
-      </c>
-      <c r="E31" t="str">
-        <v>Whitefield Road</v>
-      </c>
-      <c r="F31">
-        <v>5</v>
-      </c>
-      <c r="G31" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H31" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="str">
-        <v>Noah Sports Store</v>
-      </c>
-      <c r="B32" t="str">
-        <v>support@noahsports.in</v>
-      </c>
-      <c r="C32" t="str">
-        <v>https://noahsports.in/</v>
-      </c>
-      <c r="D32" t="str">
-        <v>sports</v>
-      </c>
-      <c r="E32" t="str">
-        <v>HAL 2nd Stage 7th Main, Shirdi Sai Baba Mandir Rd, Bhadrappa Layout, Indiranagar</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H32" t="str">
-        <v>PENDING</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="str">
-        <v>Sorse</v>
-      </c>
-      <c r="B33" t="str">
-        <v>info@sorse.in</v>
-      </c>
-      <c r="C33" t="str">
-        <v>https://sorse.in</v>
-      </c>
-      <c r="D33" t="str">
-        <v>restaurant</v>
-      </c>
-      <c r="E33" t="str">
-        <v>Whitefield Main Road</v>
-      </c>
-      <c r="F33">
-        <v>5</v>
-      </c>
-      <c r="G33" t="str">
-        <v>COLD_LEAD</v>
-      </c>
-      <c r="H33" t="str">
         <v>PENDING</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H33"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>